<commit_message>
Updates to record outputs Code version now retrieved from git
</commit_message>
<xml_diff>
--- a/src/main/resources/valipop/planning-files/recovery-factor.xlsx
+++ b/src/main/resources/valipop/planning-files/recovery-factor.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsd4/OneDrive/cs/PhD/code/population-model/validated/src/main/resources/planning-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsd4/OneDrive/cs/PhD/code/population-model/src/main/resources/valipop/planning-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2B9C2F-25E3-DF48-B7E5-ADBA54D3D6C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="860" windowWidth="24160" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="3120" yWindow="1240" windowWidth="28080" windowHeight="19300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -53,8 +60,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,14 +103,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -115,7 +125,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -179,83 +188,136 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:f>Sheet1!$D$2:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>102.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>110.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>122.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>88.0</c:v>
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A45A-0147-A399-B67707E6E4D5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -285,83 +347,136 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:f>Sheet1!$E$2:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>115.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>104.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>125.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>102.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>76.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89.0</c:v>
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A45A-0147-A399-B67707E6E4D5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -492,7 +607,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1119,20 +1233,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1412,16 +1532,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1444,7 +1564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1465,11 +1585,15 @@
         <f>(D2-E2)^2</f>
         <v>2500</v>
       </c>
+      <c r="G2">
+        <f>ABS(D2-E2)</f>
+        <v>50</v>
+      </c>
       <c r="K2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1480,19 +1604,27 @@
         <v>0.1</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D7" si="0">B3*C3</f>
         <v>100</v>
       </c>
       <c r="E3" s="1">
         <f>ROUNDUP((SUM(D$2:D2) - SUM($E$2:E2))*$K$2 + D3, 0)</f>
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F11" si="1">(D3-E3)^2</f>
-        <v>225</v>
+        <f t="shared" ref="F3:F13" si="1">(D3-E3)^2</f>
+        <v>2500</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G13" si="2">ABS(D3-E3)</f>
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <f>(G2^2+G3^2)/(G2+G3)</f>
+        <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1503,19 +1635,26 @@
         <v>0.1</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E4" s="1">
         <f>ROUNDUP((SUM(D$2:D3) - SUM($E$2:E3))*$K$2 + D4, 0)</f>
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>121</v>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>(G4+G3)/2</f>
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1531,37 +1670,52 @@
       </c>
       <c r="E5" s="1">
         <f>ROUNDUP((SUM(D$2:D4) - SUM($E$2:E4))*$K$2 + D5, 0)</f>
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H19" si="3">(G5+G4)/2</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="C6">
         <v>0.1</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E6" s="1">
         <f>ROUNDUP((SUM(D$2:D5) - SUM($E$2:E5))*$K$2 + D6, 0)</f>
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1577,37 +1731,52 @@
       </c>
       <c r="E7" s="1">
         <f>ROUNDUP((SUM(D$2:D6) - SUM($E$2:E6))*$K$2 + D7, 0)</f>
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1220</v>
+        <v>1000</v>
       </c>
       <c r="C8">
         <v>0.1</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="E8" s="1">
         <f>ROUNDUP((SUM(D$2:D7) - SUM($E$2:E7))*$K$2 + D8, 0)</f>
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1618,76 +1787,341 @@
         <v>0.1</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E9" s="1">
         <f>ROUNDUP((SUM(D$2:D8) - SUM($E$2:E8))*$K$2 + D9, 0)</f>
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="C10">
         <v>0.1</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="E10" s="1">
         <f>ROUNDUP((SUM(D$2:D9) - SUM($E$2:E9))*$K$2 + D10, 0)</f>
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>880</v>
+        <v>1000</v>
       </c>
       <c r="C11">
         <v>0.1</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E11" s="1">
         <f>ROUNDUP((SUM(D$2:D10) - SUM($E$2:E10))*$K$2 + D11, 0)</f>
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+      <c r="C12">
+        <v>0.1</v>
+      </c>
       <c r="D12">
-        <f t="shared" ref="D12:E12" si="2">SUM(D2:D11)</f>
-        <v>997</v>
-      </c>
-      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="E12" s="1">
+        <f>ROUNDUP((SUM(D$2:D11) - SUM($E$2:E11))*$K$2 + D12, 0)</f>
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="2"/>
-        <v>997</v>
-      </c>
-      <c r="F12">
-        <f>SUM(F2:F11)</f>
-        <v>2966</v>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1000</v>
+      </c>
+      <c r="C13">
+        <v>0.1</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13" s="1">
+        <f>ROUNDUP((SUM(D$2:D12) - SUM($E$2:E12))*$K$2 + D13, 0)</f>
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1000</v>
+      </c>
+      <c r="C14">
+        <v>0.1</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14" s="1">
+        <f>ROUNDUP((SUM(D$2:D13) - SUM($E$2:E13))*$K$2 + D14, 0)</f>
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F19" si="4">(D14-E14)^2</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G19" si="5">ABS(D14-E14)</f>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1000</v>
+      </c>
+      <c r="C15">
+        <v>0.1</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15" s="1">
+        <f>ROUNDUP((SUM(D$2:D14) - SUM($E$2:E14))*$K$2 + D15, 0)</f>
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1000</v>
+      </c>
+      <c r="C16">
+        <v>0.1</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16" s="1">
+        <f>ROUNDUP((SUM(D$2:D15) - SUM($E$2:E15))*$K$2 + D16, 0)</f>
+        <v>100</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F19" si="6">(D16-E16)^2</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G19" si="7">ABS(D16-E16)</f>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1000</v>
+      </c>
+      <c r="C17">
+        <v>0.1</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1">
+        <f>ROUNDUP((SUM(D$2:D16) - SUM($E$2:E16))*$K$2 + D17, 0)</f>
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1000</v>
+      </c>
+      <c r="C18">
+        <v>0.1</v>
+      </c>
+      <c r="D18">
+        <v>100</v>
+      </c>
+      <c r="E18" s="1">
+        <f>ROUNDUP((SUM(D$2:D17) - SUM($E$2:E17))*$K$2 + D18, 0)</f>
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1000</v>
+      </c>
+      <c r="C19">
+        <v>0.1</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="E19" s="1">
+        <f>ROUNDUP((SUM(D$2:D18) - SUM($E$2:E18))*$K$2 + D19, 0)</f>
+        <v>100</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="D20">
+        <f t="shared" ref="D20:E20" si="8">SUM(D2:D13)</f>
+        <v>1200</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="8"/>
+        <v>1200</v>
+      </c>
+      <c r="F20">
+        <f>SUM(F2:F13)</f>
+        <v>5000</v>
+      </c>
+      <c r="H20">
+        <f>SUM(H3:H13)</f>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>